<commit_message>
double counting on vantage_other_funds
</commit_message>
<xml_diff>
--- a/financial report data.xlsx
+++ b/financial report data.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cl\Documents\Python Scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cl\Documents\HL_model_git\HL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="revenue" sheetId="1" r:id="rId1"/>
     <sheet name="costs" sheetId="2" r:id="rId2"/>
     <sheet name="aua" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -488,7 +488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
@@ -1750,8 +1750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91C809BF-76D5-4F5B-86EC-054407FAFF76}">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1827,7 +1827,7 @@
         <v>42916</v>
       </c>
       <c r="B3" s="3">
-        <v>3465000000</v>
+        <v>3365000000</v>
       </c>
       <c r="C3" s="3">
         <v>35000000</v>
@@ -1842,13 +1842,13 @@
         <v>3400000000</v>
       </c>
       <c r="G3" s="3">
-        <v>19799000000</v>
+        <v>21581000000</v>
       </c>
       <c r="H3" s="3">
-        <v>39368000000</v>
+        <v>37092000000</v>
       </c>
       <c r="I3" s="3">
-        <v>7733000000</v>
+        <v>8327000000</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>